<commit_message>
fixed the mis-writing for Pythonic Development IDE in IDE column, modified FaceBook to Meta because they renamed recently, also fixed a few mis-spelling errors
</commit_message>
<xml_diff>
--- a/01. UI框架对比.xlsx
+++ b/01. UI框架对比.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ui-framework-comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E470338D-F8B3-40E2-8B0A-A025FD14FE5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381F0AD7-E8F5-44D5-98CF-E3F7FE4AD75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -253,14 +253,6 @@
     <t>Qt Company</t>
   </si>
   <si>
-    <t>开源社区
-W3C Organization
-Google
-FackBook
-（难得有竞争对手为同一个技术站台）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>是否支持高DPI拉伸</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -285,9 +277,6 @@
   <si>
     <t>Visual Studio/VS Code/PyCharm/Jupyter Notebook</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Visual Studio/VS Code</t>
   </si>
   <si>
     <t>Visual Studio/VS Code</t>
@@ -392,17 +381,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">
-而如果是开源社区，虽然不至于抛弃
-（社区是众多开发者构成的，
-没有人有权利终止一个项目），
-但也可能不温不火没人用。
-e.g. wxWidgets
-如果是开源 + 公司撑腰，
-那就很棒。e.g. 网页</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">开源框架有个好处：
 在撑腰的人抛弃之后，
 如果用的人多，这些开发者
@@ -420,13 +398,6 @@
 BloodSheild抛弃，
 国内大佬使用源码
 继续更新，最近4年一直更新不间断</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>如果是公司撑腰，有被抛弃的风险，
-在加上大多数公司从来不开源，
-抛弃后即使开发者众多，
-也无法志愿维护。e.g. WinForm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -482,12 +453,78 @@
 但大家不放心用，毕竟是微软出的。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Visual Studio/VS Code/PyCharm/Jupyter Notebook</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">开源社区
+W3C Organization
+Google
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FackBook</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Meta
+Microsoft (最近开始支持)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+（难得有竞争对手为同一个技术站台）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如果是公司撑腰，有被抛弃的风险，
+再加上大多数公司从来不开源，
+抛弃后即使开发者众多，
+也无法志愿维护。e.g. WinForm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+而如果是开源社区，虽然不至于被抛弃
+（社区是众多开发者构成的，
+没有人有权利终止一个项目），
+但也可能不温不火没人用。
+e.g. wxWidgets
+如果是开源 + 公司撑腰，
+那就很棒。e.g. 网页</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -497,6 +534,23 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -617,12 +671,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -631,6 +679,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -914,11 +968,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="J21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L21" sqref="L21"/>
+      <selection pane="bottomRight" activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -949,13 +1003,13 @@
         <v>20</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>27</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>39</v>
@@ -988,7 +1042,7 @@
         <v>25</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7" t="s">
@@ -1013,7 +1067,7 @@
         <v>25</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8" t="s">
@@ -1042,13 +1096,13 @@
         <v>24</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>25</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>40</v>
@@ -1077,13 +1131,13 @@
         <v>24</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>40</v>
@@ -1116,7 +1170,7 @@
         <v>25</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7" t="s">
@@ -1143,7 +1197,7 @@
         <v>26</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8" t="s">
@@ -1174,13 +1228,13 @@
         <v>22</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7" t="s">
@@ -1207,7 +1261,7 @@
         <v>28</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8" t="s">
@@ -1236,13 +1290,13 @@
         <v>21</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7" t="s">
@@ -1254,36 +1308,36 @@
       </c>
     </row>
     <row r="11" spans="1:15" s="5" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="12" t="s">
-        <v>59</v>
+      <c r="E11" s="16" t="s">
+        <v>58</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="K11" s="13" t="s">
-        <v>57</v>
+      <c r="K11" s="15" t="s">
+        <v>88</v>
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
@@ -1291,228 +1345,228 @@
       <c r="O11" s="4"/>
     </row>
     <row r="12" spans="1:15" s="5" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="12"/>
+      <c r="E12" s="16"/>
       <c r="F12" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
+        <v>87</v>
+      </c>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
     </row>
     <row r="13" spans="1:15" s="5" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="12"/>
+      <c r="E13" s="16"/>
       <c r="F13" s="8" t="s">
         <v>25</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
+        <v>60</v>
+      </c>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
     </row>
     <row r="14" spans="1:15" s="5" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
       <c r="D14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="12"/>
+      <c r="E14" s="16"/>
       <c r="F14" s="8" t="s">
         <v>28</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
+        <v>64</v>
+      </c>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
     </row>
     <row r="15" spans="1:15" s="5" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
       <c r="D15" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="12"/>
+      <c r="E15" s="16"/>
       <c r="F15" s="8" t="s">
         <v>35</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
+        <v>65</v>
+      </c>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
     </row>
     <row r="16" spans="1:15" s="5" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
       <c r="D16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="12"/>
+      <c r="E16" s="16"/>
       <c r="F16" s="8" t="s">
         <v>36</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
+        <v>64</v>
+      </c>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
     </row>
     <row r="17" spans="1:15" s="5" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
       <c r="D17" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="12"/>
+      <c r="E17" s="16"/>
       <c r="F17" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
     </row>
     <row r="18" spans="1:15" s="5" customFormat="1" ht="42.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="16"/>
+      <c r="F18" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
     </row>
-    <row r="19" spans="1:15" s="15" customFormat="1" ht="125.65" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="15" t="s">
+    <row r="19" spans="1:15" s="13" customFormat="1" ht="125.65" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="D19" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="F19" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H19" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="I19" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="J19" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="F19" s="16" t="s">
+      <c r="K19" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" s="13" customFormat="1" ht="163.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="K20" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="G19" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="I19" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="J19" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="K19" s="16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" s="15" customFormat="1" ht="163.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="J20" s="16" t="s">
+    </row>
+    <row r="21" spans="1:15" s="13" customFormat="1" ht="266.64999999999998" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="K20" s="16" t="s">
+      <c r="K21" s="14" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" s="15" customFormat="1" ht="266.64999999999998" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="K21" s="16" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="14.25" thickTop="1" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
fixed the style of the sheet
</commit_message>
<xml_diff>
--- a/01. UI框架对比.xlsx
+++ b/01. UI框架对比.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ui-framework-comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381F0AD7-E8F5-44D5-98CF-E3F7FE4AD75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75F59D7-D3E7-4493-ADE8-56F4CAC89A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -640,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -684,6 +684,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -968,11 +974,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J21" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K23" sqref="K23"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1483,27 +1489,27 @@
       <c r="O17" s="4"/>
     </row>
     <row r="18" spans="1:15" s="5" customFormat="1" ht="42.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
       <c r="D18" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="16"/>
+      <c r="E18" s="18"/>
       <c r="F18" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
     </row>
-    <row r="19" spans="1:15" s="13" customFormat="1" ht="125.65" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" s="17" customFormat="1" ht="125.65" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="13" t="s">
         <v>71</v>
       </c>
@@ -1538,19 +1544,24 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="13" customFormat="1" ht="163.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:15" s="17" customFormat="1" ht="163.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="13" t="s">
         <v>71</v>
       </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
       <c r="D20" s="14" t="s">
         <v>79</v>
       </c>
+      <c r="E20" s="13"/>
       <c r="F20" s="14" t="s">
         <v>85</v>
       </c>
       <c r="G20" s="14" t="s">
         <v>83</v>
       </c>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
       <c r="J20" s="14" t="s">
         <v>81</v>
       </c>
@@ -1558,13 +1569,21 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="13" customFormat="1" ht="266.64999999999998" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:15" s="17" customFormat="1" ht="266.64999999999998" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="13" t="s">
         <v>71</v>
       </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
       <c r="F21" s="14" t="s">
         <v>84</v>
       </c>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
       <c r="K21" s="14" t="s">
         <v>90</v>
       </c>

</xml_diff>

<commit_message>
modified the size of the excel sheet and make it printable as a pdf
</commit_message>
<xml_diff>
--- a/01. UI框架对比.xlsx
+++ b/01. UI框架对比.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ui-framework-comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75F59D7-D3E7-4493-ADE8-56F4CAC89A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CBA2B5-E10E-4839-9CD3-2D54E8652D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -640,18 +640,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -680,13 +674,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -972,13 +966,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -992,603 +986,550 @@
     <col min="9" max="9" width="56.796875" style="1" customWidth="1"/>
     <col min="10" max="10" width="32.86328125" style="1" customWidth="1"/>
     <col min="11" max="11" width="35.1328125" style="1" customWidth="1"/>
-    <col min="12" max="15" width="25.59765625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-    </row>
-    <row r="2" spans="1:15" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="7" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="7" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7" t="s">
+      <c r="J2" s="5"/>
+      <c r="K2" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="5" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:11" s="3" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="8" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8" t="s">
+      <c r="J3" s="6"/>
+      <c r="K3" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-    </row>
-    <row r="4" spans="1:15" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="7" t="s">
+    </row>
+    <row r="4" spans="1:11" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="5" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:11" s="3" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-    </row>
-    <row r="6" spans="1:15" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="7" t="s">
+    </row>
+    <row r="6" spans="1:11" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="7" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7" t="s">
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7" t="s">
+      <c r="H6" s="5"/>
+      <c r="I6" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="5" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:11" s="3" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="8" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8" t="s">
+      <c r="H7" s="6"/>
+      <c r="I7" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-    </row>
-    <row r="8" spans="1:15" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="7" t="s">
+    </row>
+    <row r="8" spans="1:11" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7" t="s">
+      <c r="H8" s="5"/>
+      <c r="I8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="K8" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="5" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:11" s="3" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="8" t="s">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8" t="s">
+      <c r="E9" s="6"/>
+      <c r="F9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8" t="s">
+      <c r="H9" s="6"/>
+      <c r="I9" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8" t="s">
+      <c r="J9" s="6"/>
+      <c r="K9" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-    </row>
-    <row r="10" spans="1:15" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="7" t="s">
+    </row>
+    <row r="10" spans="1:11" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7" t="s">
+      <c r="H10" s="5"/>
+      <c r="I10" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7" t="s">
+      <c r="J10" s="5"/>
+      <c r="K10" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="5" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="16" t="s">
+    <row r="11" spans="1:11" s="3" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16" t="s">
+      <c r="H11" s="15"/>
+      <c r="I11" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="J11" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-    </row>
-    <row r="12" spans="1:15" s="5" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="8" t="s">
+    </row>
+    <row r="12" spans="1:11" s="3" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="8" t="s">
+      <c r="E12" s="15"/>
+      <c r="F12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-    </row>
-    <row r="13" spans="1:15" s="5" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="8" t="s">
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+    </row>
+    <row r="13" spans="1:11" s="3" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="8" t="s">
+      <c r="E13" s="15"/>
+      <c r="F13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-    </row>
-    <row r="14" spans="1:15" s="5" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="8" t="s">
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+    </row>
+    <row r="14" spans="1:11" s="3" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="8" t="s">
+      <c r="E14" s="15"/>
+      <c r="F14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-    </row>
-    <row r="15" spans="1:15" s="5" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="8" t="s">
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+    </row>
+    <row r="15" spans="1:11" s="3" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="8" t="s">
+      <c r="E15" s="15"/>
+      <c r="F15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-    </row>
-    <row r="16" spans="1:15" s="5" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="8" t="s">
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+    </row>
+    <row r="16" spans="1:11" s="3" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="8" t="s">
+      <c r="E16" s="15"/>
+      <c r="F16" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-    </row>
-    <row r="17" spans="1:15" s="5" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="8" t="s">
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+    </row>
+    <row r="17" spans="1:11" s="3" customFormat="1" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="9" t="s">
+      <c r="E17" s="15"/>
+      <c r="F17" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="G17" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-    </row>
-    <row r="18" spans="1:15" s="5" customFormat="1" ht="42.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="12" t="s">
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+    </row>
+    <row r="18" spans="1:11" s="3" customFormat="1" ht="42.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="18"/>
-      <c r="F18" s="12" t="s">
+      <c r="E18" s="16"/>
+      <c r="F18" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-    </row>
-    <row r="19" spans="1:15" s="17" customFormat="1" ht="125.65" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="13" t="s">
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+    </row>
+    <row r="19" spans="1:11" s="13" customFormat="1" ht="125.65" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="H19" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="I19" s="14" t="s">
+      <c r="I19" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="J19" s="14" t="s">
+      <c r="J19" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="K19" s="14" t="s">
+      <c r="K19" s="12" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="17" customFormat="1" ht="163.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="13" t="s">
+    <row r="20" spans="1:11" s="13" customFormat="1" ht="163.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="14" t="s">
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="14" t="s">
+      <c r="E20" s="11"/>
+      <c r="F20" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="14" t="s">
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="K20" s="14" t="s">
+      <c r="K20" s="12" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="17" customFormat="1" ht="266.64999999999998" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="13" t="s">
+    <row r="21" spans="1:11" s="13" customFormat="1" ht="266.64999999999998" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="14" t="s">
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="14" t="s">
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="12" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="14.25" thickTop="1" x14ac:dyDescent="0.4"/>
+    <row r="22" spans="1:11" ht="14.25" thickTop="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="K11:K18"/>
@@ -1602,7 +1543,7 @@
     <mergeCell ref="I11:I18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="60" fitToWidth="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>